<commit_message>
fix file excel KETOAN-BACHKHOA ==> HOADON-BACHKHOA
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportDanhMuc/Danh_Muc_Hang_Hoa_Dich_Vu_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportDanhMuc/Danh_Muc_Hang_Hoa_Dich_Vu_Import.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RD-Thien\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="KETOAN-BACHKHOA" sheetId="1" r:id="rId1"/>
@@ -435,23 +435,23 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="6" customWidth="1"/>
     <col min="7" max="7" width="22" style="8" customWidth="1"/>
-    <col min="8" max="8" width="37.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="37.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -479,8 +479,8 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADONBACHKHOA" prompt="Giá bán là đơn giá sau thuế. _x000a_- Chọn 0 : Giá bán không phải là đơn giá sau thuế_x000a_- Chọn 1 : Giá bán là đơn giá sau thuế" sqref="E1:E1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADONBACHKHOA" prompt="Thuế GTGT (%)_x000a_- Thuế suất 0%, 5%, 10%: điền giá trị tương ứng 0, 5, 10_x000a_- Không chịu thuế: điền giá trị KCT_x000a_- Không kê khai nộp thuế: điền giá trị KKKNT_x000a_- TH Khác: KHAC" sqref="F1:F1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Giá bán là đơn giá sau thuế. _x000a_- Chọn 0 : Giá bán không phải là đơn giá sau thuế_x000a_- Chọn 1 : Giá bán là đơn giá sau thuế" sqref="E1:E1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Thuế GTGT (%)_x000a_- Thuế suất 0%, 5%, 10%: điền giá trị tương ứng 0, 5, 10_x000a_- Không chịu thuế: điền giá trị KCT_x000a_- Không kê khai nộp thuế: điền giá trị KKKNT_x000a_- TH Khác: KHAC" sqref="F1:F1048576"/>
   </dataValidations>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.39370078740157483" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.23622047244094491"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fix lấy nhật ký mẫu hóa đơn và file excel
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportDanhMuc/Danh_Muc_Hang_Hoa_Dich_Vu_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportDanhMuc/Danh_Muc_Hang_Hoa_Dich_Vu_Import.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanlt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12144"/>
   </bookViews>
   <sheets>
-    <sheet name="KETOAN-BACHKHOA" sheetId="1" r:id="rId1"/>
+    <sheet name="HOADON-BACHKHOA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -435,7 +435,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>